<commit_message>
Changed vertical DB2EVC-2.54-2P-GN to right angle DB2ERC-2.54-2P-GN Changed vertical DB2EVC-2.54-3P-GN to right angle DB2ERC-2.54-3P-GN Add plugs for 2.54mm
</commit_message>
<xml_diff>
--- a/Project Outputs for Longboard_32bit/BOM/JLPCB BOM-Longboard_32bit_A4_FULL_PLACE.xlsx
+++ b/Project Outputs for Longboard_32bit/BOM/JLPCB BOM-Longboard_32bit_A4_FULL_PLACE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sienci\Repos\longboard_stm32\Project Outputs for Longboard_32bit\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B259EAD3-7B93-4DCE-B6FB-154066DA6E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF60C19B-3AF1-4082-B584-ED60FC980921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="82860" yWindow="1575" windowWidth="28800" windowHeight="15195" xr2:uid="{51C0715C-6756-4056-A71E-D328EAECD22B}"/>
+    <workbookView xWindow="84855" yWindow="2715" windowWidth="28800" windowHeight="15195" xr2:uid="{025E5B45-9C53-4A90-ADE1-FA5BA6877C6E}"/>
   </bookViews>
   <sheets>
     <sheet name="JLPCB BOM-Longboard_32bit_A4_FU" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="451">
   <si>
     <t>Quantity</t>
   </si>
@@ -444,28 +444,28 @@
     <t>J1</t>
   </si>
   <si>
-    <t>DB2EVC-2.54-3P-GN</t>
+    <t>DB2ERC-2.54-3P-GN</t>
   </si>
   <si>
     <t>DIBO</t>
   </si>
   <si>
-    <t>150V 5A 3 Straight pin -40℃~+105℃ Copper Alloy 1 2.54mm Green Board Edge/Receptacle-Close Tin Straight,P=2.54mm Pluggable System Terminal Block ROHS</t>
-  </si>
-  <si>
-    <t>C2927494</t>
+    <t>150V 5A 3 Bend -40℃~+105℃ Copper Alloy 1 2.54mm Green Board Edge/Receptacle-Close Tin Push-Pull,P=2.54mm Pluggable System Terminal Block ROHS</t>
+  </si>
+  <si>
+    <t>C2927504</t>
   </si>
   <si>
     <t>J2</t>
   </si>
   <si>
-    <t>DB2EVC-2.54-2P-GN</t>
-  </si>
-  <si>
-    <t>150V 5A 2 Straight pin -40℃~+105℃ Copper Alloy 1 2.54mm Green Board Edge/Receptacle-Close Tin Straight,P=2.54mm Pluggable System Terminal Block ROHS</t>
-  </si>
-  <si>
-    <t>C2927493</t>
+    <t>DB2ERC-2.54-2P-GN</t>
+  </si>
+  <si>
+    <t>150V 5A 2 Bend -40℃~+105℃ Copper Alloy 1 2.54mm Green Board Edge/Receptacle-Close Tin Push-Pull,P=2.54mm Pluggable System Terminal Block ROHS</t>
+  </si>
+  <si>
+    <t>C2927503</t>
   </si>
   <si>
     <t>J3, J13</t>
@@ -669,6 +669,18 @@
     <t>J29, J30</t>
   </si>
   <si>
+    <t>DB2EK-2.54-2P-GN-S</t>
+  </si>
+  <si>
+    <t>150V 5A 2 -40℃~+105℃ Copper Alloy 1 2.54mm Green Plug Tin P=2.54mm Pluggable System Terminal Block ROHS</t>
+  </si>
+  <si>
+    <t>C2927483</t>
+  </si>
+  <si>
+    <t>J35, J36</t>
+  </si>
+  <si>
     <t>Ferrite Bead</t>
   </si>
   <si>
@@ -757,6 +769,18 @@
   </si>
   <si>
     <t>WJ15EDGRC-3.81-2P</t>
+  </si>
+  <si>
+    <t>DB2EK-2.54-3P-GN-S</t>
+  </si>
+  <si>
+    <t>150V 5A 3 -40℃~+105℃ Copper Alloy 1 2.54mm Green Plug Tin P=2.54mm Pluggable System Terminal Block ROHS</t>
+  </si>
+  <si>
+    <t>C2927484</t>
+  </si>
+  <si>
+    <t>P7</t>
   </si>
   <si>
     <t>PZ254V-12-8P</t>
@@ -1741,8 +1765,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9BB654-1586-49F0-A2A4-AB2DBC154736}">
-  <dimension ref="A1:G109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863AD3DD-7155-48D3-937F-8CD7303364FE}">
+  <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2827,26 +2851,30 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>6</v>
-      </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="D51" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2865,7 +2893,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2884,25 +2912,21 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>1</v>
-      </c>
-      <c r="B54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2910,87 +2934,87 @@
         <v>1</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="G55" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>6</v>
-      </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="D57" s="2" t="s">
-        <v>150</v>
+        <v>238</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>4</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2998,52 +3022,54 @@
         <v>1</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="G59" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>1</v>
       </c>
-      <c r="B61" s="1"/>
+      <c r="B61" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="C61" s="2" t="s">
         <v>255</v>
       </c>
@@ -3057,27 +3083,27 @@
         <v>258</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>259</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>199</v>
+        <v>260</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>259</v>
@@ -3085,11 +3111,9 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>2</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>262</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B63" s="1"/>
       <c r="C63" s="2" t="s">
         <v>263</v>
       </c>
@@ -3103,27 +3127,27 @@
         <v>266</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="F64" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>267</v>
@@ -3131,275 +3155,279 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>7</v>
-      </c>
-      <c r="B65" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>270</v>
+      </c>
       <c r="C65" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="G65" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>11</v>
-      </c>
-      <c r="B66" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="C66" s="2" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3408,19 +3436,19 @@
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3429,166 +3457,166 @@
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3597,63 +3625,61 @@
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>2</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>343</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B89" s="1"/>
       <c r="C89" s="2" t="s">
-        <v>344</v>
+        <v>280</v>
       </c>
       <c r="D89" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="F89" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="G89" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3662,65 +3688,63 @@
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="E91" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="F91" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>357</v>
-      </c>
       <c r="G91" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>41</v>
-      </c>
-      <c r="B92" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="1"/>
+      <c r="C92" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="F92" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="G92" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3728,30 +3752,34 @@
         <v>1</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="E93" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>367</v>
-      </c>
       <c r="G93" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>1</v>
-      </c>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>367</v>
+      </c>
       <c r="D94" s="2" t="s">
         <v>368</v>
       </c>
@@ -3762,133 +3790,129 @@
         <v>370</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>1</v>
       </c>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
+      <c r="B95" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="D95" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>1</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="E96" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="F96" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="G96" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E97" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="F97" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="G97" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>1</v>
       </c>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
+      <c r="B98" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="D98" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>1</v>
-      </c>
-      <c r="B99" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="E99" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>1</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E100" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3896,22 +3920,22 @@
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="E101" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>403</v>
-      </c>
       <c r="G101" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3919,29 +3943,31 @@
         <v>1</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D102" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D102" s="2" t="s">
+      <c r="E102" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="F102" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="G102" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>1</v>
       </c>
-      <c r="B103" s="1"/>
+      <c r="B103" s="2" t="s">
+        <v>407</v>
+      </c>
       <c r="C103" s="2" t="s">
         <v>408</v>
       </c>
@@ -3955,15 +3981,19 @@
         <v>411</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>1</v>
       </c>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
+      <c r="B104" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>408</v>
+      </c>
       <c r="D104" s="2" t="s">
         <v>413</v>
       </c>
@@ -3974,53 +4004,47 @@
         <v>415</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>1</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" s="1"/>
+      <c r="C105" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D105" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="E105" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="F105" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E105" s="2" t="s">
+      <c r="G105" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>1</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E106" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="F106" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="G106" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4028,22 +4052,22 @@
         <v>1</v>
       </c>
       <c r="B107" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D107" s="2" t="s">
+      <c r="E107" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E107" s="2" t="s">
+      <c r="F107" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="F107" s="2" t="s">
-        <v>430</v>
-      </c>
       <c r="G107" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4051,22 +4075,22 @@
         <v>1</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="D108" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="E108" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="E108" s="2" t="s">
+      <c r="F108" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="F108" s="2" t="s">
-        <v>435</v>
-      </c>
       <c r="G108" s="2" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4074,22 +4098,68 @@
         <v>1</v>
       </c>
       <c r="B109" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E109" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="F109" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="G109" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>1</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="E109" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="D110" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="G109" s="2" t="s">
+      <c r="E110" s="2" t="s">
         <v>442</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>1</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fill out MFG and MFG Part Numbers
</commit_message>
<xml_diff>
--- a/Project Outputs for Longboard_32bit/BOM/JLPCB BOM-Longboard_32bit_A4_FULL_PLACE.xlsx
+++ b/Project Outputs for Longboard_32bit/BOM/JLPCB BOM-Longboard_32bit_A4_FULL_PLACE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sienci\Repos\longboard_stm32\Project Outputs for Longboard_32bit\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF60C19B-3AF1-4082-B584-ED60FC980921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{546D7A82-C289-42EC-B9F7-9585D5359C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84855" yWindow="2715" windowWidth="28800" windowHeight="15195" xr2:uid="{025E5B45-9C53-4A90-ADE1-FA5BA6877C6E}"/>
+    <workbookView xWindow="84855" yWindow="2715" windowWidth="28800" windowHeight="15195" xr2:uid="{5CB1C09F-25AA-42A5-9CE5-4242CA91869C}"/>
   </bookViews>
   <sheets>
     <sheet name="JLPCB BOM-Longboard_32bit_A4_FU" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="510">
   <si>
     <t>Quantity</t>
   </si>
@@ -60,6 +60,9 @@
     <t>Comment</t>
   </si>
   <si>
+    <t>CC0603KRX7R9BB104</t>
+  </si>
+  <si>
     <t>YAGEO</t>
   </si>
   <si>
@@ -75,6 +78,9 @@
     <t>100nF</t>
   </si>
   <si>
+    <t>CL10A105KB8NNNC</t>
+  </si>
+  <si>
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
@@ -87,6 +93,9 @@
     <t>1uF</t>
   </si>
   <si>
+    <t>CL31A106KBHNNNE</t>
+  </si>
+  <si>
     <t>C13585</t>
   </si>
   <si>
@@ -96,6 +105,9 @@
     <t>10uF</t>
   </si>
   <si>
+    <t>CL21A475KAQNNNE</t>
+  </si>
+  <si>
     <t>C1779</t>
   </si>
   <si>
@@ -105,6 +117,9 @@
     <t>4.7uF</t>
   </si>
   <si>
+    <t>CL21A226MAQNNNE</t>
+  </si>
+  <si>
     <t>C45783</t>
   </si>
   <si>
@@ -114,6 +129,9 @@
     <t>22uF</t>
   </si>
   <si>
+    <t>0603B103K500NT</t>
+  </si>
+  <si>
     <t>Guangdong Fenghua Advanced Tech</t>
   </si>
   <si>
@@ -126,6 +144,9 @@
     <t>10nF</t>
   </si>
   <si>
+    <t>CL10C100JB8NNNC</t>
+  </si>
+  <si>
     <t>C1634</t>
   </si>
   <si>
@@ -135,6 +156,9 @@
     <t>10pF</t>
   </si>
   <si>
+    <t>CC0603KRX7R9BB822</t>
+  </si>
+  <si>
     <t>50V 8.2nF X7R ±10% 0603 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
@@ -147,12 +171,18 @@
     <t>8.2nF</t>
   </si>
   <si>
+    <t>CL10A475KO8NNNC</t>
+  </si>
+  <si>
     <t>C19666</t>
   </si>
   <si>
     <t>C23, C25, C26, C54, C84, C88, C91</t>
   </si>
   <si>
+    <t>CL10B224KA8NNNC</t>
+  </si>
+  <si>
     <t>C21120</t>
   </si>
   <si>
@@ -180,12 +210,18 @@
     <t>220uF</t>
   </si>
   <si>
+    <t>CL21A106KAYNNNE</t>
+  </si>
+  <si>
     <t>C15850</t>
   </si>
   <si>
     <t>C48_STEP_A, C48_STEP_X, C48_STEP_Y, C48_STEP_Z</t>
   </si>
   <si>
+    <t>CL10B474KA8NNNC</t>
+  </si>
+  <si>
     <t>C1623</t>
   </si>
   <si>
@@ -195,6 +231,9 @@
     <t>470nF</t>
   </si>
   <si>
+    <t>TAJB107K006RNJ</t>
+  </si>
+  <si>
     <t>AVX</t>
   </si>
   <si>
@@ -210,6 +249,9 @@
     <t>100uF</t>
   </si>
   <si>
+    <t>HV101M035E077ETR</t>
+  </si>
+  <si>
     <t>Capxon International Elec</t>
   </si>
   <si>
@@ -249,6 +291,12 @@
     <t>Raspberry Pi Compute Module 4-B</t>
   </si>
   <si>
+    <t>19-217/GHC-YR1S2/3T</t>
+  </si>
+  <si>
+    <t>Everlight Elec</t>
+  </si>
+  <si>
     <t>LED</t>
   </si>
   <si>
@@ -264,9 +312,6 @@
     <t>19-213SURC/S530-A3/TR8</t>
   </si>
   <si>
-    <t>Everlight Elec</t>
-  </si>
-  <si>
     <t>20mA 632nm Colorless transparence 624nm~624nm -40℃~+85℃ Red 120° 60mW 0603 Light Emitting Diodes (LED) ROHS</t>
   </si>
   <si>
@@ -279,6 +324,9 @@
     <t>0603 Red</t>
   </si>
   <si>
+    <t>19-213/Y2C-CQ2R2L/3T(CY)</t>
+  </si>
+  <si>
     <t>C72038</t>
   </si>
   <si>
@@ -288,6 +336,12 @@
     <t>0603 Yellow</t>
   </si>
   <si>
+    <t>SM712</t>
+  </si>
+  <si>
+    <t>DOWO</t>
+  </si>
+  <si>
     <t>Bidirectional 12V (Max), 7V (Max) 7.5V / 13.3V 10V / 20V 12A(8/20us) SOT-23-3 TVS RoHS</t>
   </si>
   <si>
@@ -297,7 +351,7 @@
     <t>D14, D16</t>
   </si>
   <si>
-    <t>SM712</t>
+    <t>19-217UWD/S365-2/TR8</t>
   </si>
   <si>
     <t>C133759</t>
@@ -324,6 +378,12 @@
     <t>D19</t>
   </si>
   <si>
+    <t>SMAZ27-13-F</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
     <t>27V ±5% 1W 500nA @ 20.5V SMA(DO-214AC) Zener Diodes RoHS</t>
   </si>
   <si>
@@ -333,9 +393,6 @@
     <t>D21</t>
   </si>
   <si>
-    <t>SMAZ27-13-F</t>
-  </si>
-  <si>
     <t>SSB43L-E3/52T</t>
   </si>
   <si>
@@ -354,15 +411,18 @@
     <t>SSB43L-E3_52T</t>
   </si>
   <si>
+    <t>1SMAF4734A</t>
+  </si>
+  <si>
+    <t>Shandong Jingdao Microelectronics</t>
+  </si>
+  <si>
     <t>C169539</t>
   </si>
   <si>
     <t>D23</t>
   </si>
   <si>
-    <t>1SMAF4734A</t>
-  </si>
-  <si>
     <t>USBLC6-2SC6</t>
   </si>
   <si>
@@ -378,6 +438,12 @@
     <t>D27</t>
   </si>
   <si>
+    <t>SS36-E3/57T</t>
+  </si>
+  <si>
+    <t>Vishay Intertech</t>
+  </si>
+  <si>
     <t>DIODE SCHOTTKY 60V 3A DO214AB</t>
   </si>
   <si>
@@ -387,7 +453,10 @@
     <t>D28</t>
   </si>
   <si>
-    <t>SS36-E3/57T</t>
+    <t>B5819W SL</t>
+  </si>
+  <si>
+    <t>Jiangsu Changjing Electronics Technology</t>
   </si>
   <si>
     <t>Schottky Diode</t>
@@ -402,6 +471,9 @@
     <t>B5819W  SL</t>
   </si>
   <si>
+    <t>JK-nSMD050-24</t>
+  </si>
+  <si>
     <t>Jinrui Electronic Materials Co.</t>
   </si>
   <si>
@@ -417,6 +489,12 @@
     <t>24V 1A</t>
   </si>
   <si>
+    <t>TMC2660C-PA-T</t>
+  </si>
+  <si>
+    <t>TRINAMIC</t>
+  </si>
+  <si>
     <t>QFP-44 Motor Driver ICs ROHS</t>
   </si>
   <si>
@@ -426,9 +504,6 @@
     <t>IC1_STEP_A, IC1_STEP_X, IC1_STEP_Y, IC1_STEP_Z</t>
   </si>
   <si>
-    <t>TMC2660C-PA-T</t>
-  </si>
-  <si>
     <t>95278-101A16LF</t>
   </si>
   <si>
@@ -471,7 +546,7 @@
     <t>J3, J13</t>
   </si>
   <si>
-    <t>None</t>
+    <t>B3B-XH-A(LF)(SN)</t>
   </si>
   <si>
     <t>JST Sales America</t>
@@ -486,7 +561,10 @@
     <t>J4, J5, J6, J7, J8, J21</t>
   </si>
   <si>
-    <t>B3B-XH-A(LF)(SN)</t>
+    <t>WJ15EDGRC-3.81-5P</t>
+  </si>
+  <si>
+    <t>Ningbo Kangnex</t>
   </si>
   <si>
     <t>3.81mm Green Board Edge/Receptacle-Close Push-Pull,P=3.81mm Pluggable System Terminal Block ROHS</t>
@@ -498,9 +576,6 @@
     <t>J9</t>
   </si>
   <si>
-    <t>WJ15EDGRC-3.81-5P</t>
-  </si>
-  <si>
     <t>WJ15EDGRC-3.81-4P</t>
   </si>
   <si>
@@ -513,15 +588,15 @@
     <t>J10, J34</t>
   </si>
   <si>
+    <t>WJ15EDGRC-3.81-3P</t>
+  </si>
+  <si>
     <t>C8406</t>
   </si>
   <si>
     <t>J11</t>
   </si>
   <si>
-    <t>WJ15EDGRC-3.81-3P</t>
-  </si>
-  <si>
     <t>DS1133-S60BPX</t>
   </si>
   <si>
@@ -582,6 +657,12 @@
     <t>J18</t>
   </si>
   <si>
+    <t>1747981-1</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
     <t>HDMI Receptacle, Pitch 0.5 mm, 19 Position, Height 6.38 mm, RoHS, Tape and Reel</t>
   </si>
   <si>
@@ -591,7 +672,10 @@
     <t>J19</t>
   </si>
   <si>
-    <t>1747981-1</t>
+    <t>TYPE-C-31-M-12</t>
+  </si>
+  <si>
+    <t>HRO Electronics Co., Ltd.</t>
   </si>
   <si>
     <t>USB Connectors 24 Receptacle 1 8.94*7.3mm RoHS</t>
@@ -603,9 +687,6 @@
     <t>J20</t>
   </si>
   <si>
-    <t>TYPE-C-31-M-12</t>
-  </si>
-  <si>
     <t>WJ2EDGK-5.08-4P</t>
   </si>
   <si>
@@ -681,6 +762,12 @@
     <t>J35, J36</t>
   </si>
   <si>
+    <t>CBG100505U221T</t>
+  </si>
+  <si>
+    <t>FH (Guangdong Fenghua Advanced Tech)</t>
+  </si>
+  <si>
     <t>Ferrite Bead</t>
   </si>
   <si>
@@ -693,6 +780,12 @@
     <t>220R @ 100Mhz 100mA</t>
   </si>
   <si>
+    <t>YSPI0630A-220M</t>
+  </si>
+  <si>
+    <t>YJYCOIN</t>
+  </si>
+  <si>
     <t>3A 22uH ±20% 130mΩ SMD,7.1x6.6x3mm Power Inductors ROHS</t>
   </si>
   <si>
@@ -705,6 +798,9 @@
     <t>22 uH</t>
   </si>
   <si>
+    <t>CBW201209U221T</t>
+  </si>
+  <si>
     <t>220Ω @ 100MHz 1 2A 150mΩ 0805 Ferrite Beads ROHS</t>
   </si>
   <si>
@@ -762,15 +858,15 @@
     <t>P2, P3, P4, P5</t>
   </si>
   <si>
+    <t>WJ15EDGRC-3.81-2P</t>
+  </si>
+  <si>
     <t>C8387</t>
   </si>
   <si>
     <t>P6, P18_AX_RL1, P18_AX_RL2, P19, P21_AX_TR1, P21_AX_TR2</t>
   </si>
   <si>
-    <t>WJ15EDGRC-3.81-2P</t>
-  </si>
-  <si>
     <t>DB2EK-2.54-3P-GN-S</t>
   </si>
   <si>
@@ -828,6 +924,9 @@
     <t>P16, P17</t>
   </si>
   <si>
+    <t>61200821621</t>
+  </si>
+  <si>
     <t>Wurth Elektronik</t>
   </si>
   <si>
@@ -867,9 +966,6 @@
     <t>MMBT5551</t>
   </si>
   <si>
-    <t>Jiangsu Changjing Electronics Technology</t>
-  </si>
-  <si>
     <t>50nA 160V 300mW 200@10mA,5V 600mA 100MHz 200mV@50mA,5mA NPN +150℃@(Tj) SOT-23-3 Bipolar Transistors - BJT ROHS</t>
   </si>
   <si>
@@ -879,6 +975,9 @@
     <t>Q3_AX_TR1, Q3_AX_TR2</t>
   </si>
   <si>
+    <t>0603WAF0000T5E</t>
+  </si>
+  <si>
     <t>Uniroyal Elec</t>
   </si>
   <si>
@@ -894,6 +993,9 @@
     <t>0Ω ±1%</t>
   </si>
   <si>
+    <t>0603WAF2001T5E</t>
+  </si>
+  <si>
     <t>C22975</t>
   </si>
   <si>
@@ -903,6 +1005,9 @@
     <t>2KΩ ±1%</t>
   </si>
   <si>
+    <t>0603WAF1002T5E</t>
+  </si>
+  <si>
     <t>C25804</t>
   </si>
   <si>
@@ -912,6 +1017,9 @@
     <t>10KΩ ±1%</t>
   </si>
   <si>
+    <t>0603WAF1001T5E</t>
+  </si>
+  <si>
     <t>C21190</t>
   </si>
   <si>
@@ -921,6 +1029,9 @@
     <t>1KΩ ±1%</t>
   </si>
   <si>
+    <t>0603WAF4701T5E</t>
+  </si>
+  <si>
     <t>C23162</t>
   </si>
   <si>
@@ -930,6 +1041,9 @@
     <t>4.7KΩ ±1%</t>
   </si>
   <si>
+    <t>0603WAF5100T5E</t>
+  </si>
+  <si>
     <t>C23193</t>
   </si>
   <si>
@@ -939,6 +1053,9 @@
     <t>510Ω ±1%</t>
   </si>
   <si>
+    <t>0603WAF1003T5E</t>
+  </si>
+  <si>
     <t>C25803</t>
   </si>
   <si>
@@ -948,12 +1065,18 @@
     <t>100KΩ ±1%</t>
   </si>
   <si>
+    <t>0402WGF4701TCE</t>
+  </si>
+  <si>
     <t>C25900</t>
   </si>
   <si>
     <t>R33</t>
   </si>
   <si>
+    <t>0603WAF3000T5E</t>
+  </si>
+  <si>
     <t>C23025</t>
   </si>
   <si>
@@ -963,12 +1086,18 @@
     <t>300Ω ±1%</t>
   </si>
   <si>
+    <t>0402WGF5100TCE</t>
+  </si>
+  <si>
     <t>C25123</t>
   </si>
   <si>
     <t>R44, R45, R47, R50, R51, R52, R84, R88, R89</t>
   </si>
   <si>
+    <t>0603WAF5600T5E</t>
+  </si>
+  <si>
     <t>C23204</t>
   </si>
   <si>
@@ -978,6 +1107,9 @@
     <t>560Ω ±1%</t>
   </si>
   <si>
+    <t>0603WAF1300T5E</t>
+  </si>
+  <si>
     <t>C22796</t>
   </si>
   <si>
@@ -987,6 +1119,9 @@
     <t>130Ω ±1%</t>
   </si>
   <si>
+    <t>0603WAF4702T5E</t>
+  </si>
+  <si>
     <t>C25819</t>
   </si>
   <si>
@@ -996,6 +1131,9 @@
     <t>47KΩ ±1%</t>
   </si>
   <si>
+    <t>0603WAF1801T5E</t>
+  </si>
+  <si>
     <t>C4177</t>
   </si>
   <si>
@@ -1005,6 +1143,9 @@
     <t>1.8KΩ ±1%</t>
   </si>
   <si>
+    <t>0402WGF5101TCE</t>
+  </si>
+  <si>
     <t>C25905</t>
   </si>
   <si>
@@ -1014,6 +1155,9 @@
     <t>5.1KΩ ±1%</t>
   </si>
   <si>
+    <t>0402WGF2201TCE</t>
+  </si>
+  <si>
     <t>C25879</t>
   </si>
   <si>
@@ -1023,6 +1167,9 @@
     <t>2.2KΩ ±1%</t>
   </si>
   <si>
+    <t>0603WAF220JT5E</t>
+  </si>
+  <si>
     <t>C23345</t>
   </si>
   <si>
@@ -1032,6 +1179,9 @@
     <t>22Ω ±1%</t>
   </si>
   <si>
+    <t>0603WAF100JT5E</t>
+  </si>
+  <si>
     <t>C22859</t>
   </si>
   <si>
@@ -1041,6 +1191,9 @@
     <t>10Ω ±1%</t>
   </si>
   <si>
+    <t>1206W4F100LT5E</t>
+  </si>
+  <si>
     <t>C25334</t>
   </si>
   <si>
@@ -1050,12 +1203,18 @@
     <t>0.1Ω ±1%</t>
   </si>
   <si>
+    <t>0402WGF4702TCE</t>
+  </si>
+  <si>
     <t>C25792</t>
   </si>
   <si>
     <t>R86, R96, R97, R98, R99</t>
   </si>
   <si>
+    <t>0805W8F1200T5E</t>
+  </si>
+  <si>
     <t>C17437</t>
   </si>
   <si>
@@ -1065,6 +1224,9 @@
     <t>120Ω ±1%</t>
   </si>
   <si>
+    <t>0402WGF1202TCE</t>
+  </si>
+  <si>
     <t>C25752</t>
   </si>
   <si>
@@ -1074,6 +1236,9 @@
     <t>12KΩ ±1%</t>
   </si>
   <si>
+    <t>0402WGF1502TCE</t>
+  </si>
+  <si>
     <t>C25756</t>
   </si>
   <si>
@@ -1083,6 +1248,9 @@
     <t>15KΩ ±1%</t>
   </si>
   <si>
+    <t>0402WGF4700TCE</t>
+  </si>
+  <si>
     <t>C25117</t>
   </si>
   <si>
@@ -1107,6 +1275,9 @@
     <t>SD1, SD2</t>
   </si>
   <si>
+    <t>SKRTLAE010</t>
+  </si>
+  <si>
     <t>ALPS</t>
   </si>
   <si>
@@ -1119,9 +1290,6 @@
     <t>SW1, SW2</t>
   </si>
   <si>
-    <t>SKRTLAE010</t>
-  </si>
-  <si>
     <t>SN74AHC1G86DBVR</t>
   </si>
   <si>
@@ -1167,6 +1335,9 @@
     <t>U3</t>
   </si>
   <si>
+    <t>SN75176BDR</t>
+  </si>
+  <si>
     <t>RS-485/RS-422</t>
   </si>
   <si>
@@ -1176,7 +1347,7 @@
     <t>U13</t>
   </si>
   <si>
-    <t>SN75176BDR</t>
+    <t>TPS54331DR</t>
   </si>
   <si>
     <t>Switching Voltage Regulators 3A 28V In Step Down SWIFT DC/DC Cnvrtr</t>
@@ -1188,9 +1359,6 @@
     <t>U16</t>
   </si>
   <si>
-    <t>TPS54331DR</t>
-  </si>
-  <si>
     <t>STM32F412VGT6</t>
   </si>
   <si>
@@ -1206,6 +1374,9 @@
     <t>U17</t>
   </si>
   <si>
+    <t>6N137S(TA)</t>
+  </si>
+  <si>
     <t>10Mbit/s 75ns,75ns 1 -40℃~+85℃ 5000V 5kV/us DC SMD-8_6.3mm Optocouplers - Logic Output ROHS</t>
   </si>
   <si>
@@ -1215,7 +1386,10 @@
     <t>U18, U20, U27</t>
   </si>
   <si>
-    <t>6N137S(TA)</t>
+    <t>PCA82C250T/YM,118</t>
+  </si>
+  <si>
+    <t>NXP Semicon</t>
   </si>
   <si>
     <t>CAN</t>
@@ -1287,6 +1461,9 @@
     <t>U26</t>
   </si>
   <si>
+    <t>WS2812B-B/W</t>
+  </si>
+  <si>
     <t>Worldsemi</t>
   </si>
   <si>
@@ -1299,7 +1476,10 @@
     <t>U28</t>
   </si>
   <si>
-    <t>WS2812B-B/W</t>
+    <t>ZD24C128A-SSGMB</t>
+  </si>
+  <si>
+    <t>Zetta</t>
   </si>
   <si>
     <t>IC EEPROM 128KBIT I2C 8SOIC</t>
@@ -1309,9 +1489,6 @@
   </si>
   <si>
     <t>U35</t>
-  </si>
-  <si>
-    <t>ZD24C128A-SSGMB</t>
   </si>
   <si>
     <t>74LVC1G07</t>
@@ -1765,7 +1942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863AD3DD-7155-48D3-937F-8CD7303364FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514EB639-7DF3-447A-8364-0B606F89ECCF}">
   <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1808,210 +1985,230 @@
       <c r="A2" s="1">
         <v>70</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>17</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2019,106 +2216,114 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="C16" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2126,22 +2331,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2149,41 +2354,45 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2191,79 +2400,91 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>9</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="B21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="B22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="B23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2271,41 +2492,45 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="B25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2313,41 +2538,45 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="B27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2355,100 +2584,114 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="B29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D29" s="2" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="B30" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="C31" s="2" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>4</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="B32" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="D32" s="2" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2456,22 +2699,22 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2479,22 +2722,22 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2502,22 +2745,22 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2525,41 +2768,45 @@
         <v>6</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="B37" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="D37" s="2" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2567,41 +2814,45 @@
         <v>2</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="B39" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="D39" s="2" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2609,22 +2860,22 @@
         <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2632,22 +2883,22 @@
         <v>2</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2655,22 +2906,22 @@
         <v>1</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2678,60 +2929,68 @@
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="B44" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>207</v>
+      </c>
       <c r="D44" s="2" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1</v>
       </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="B45" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="D45" s="2" t="s">
-        <v>185</v>
+        <v>213</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2739,22 +2998,22 @@
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2762,22 +3021,22 @@
         <v>6</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2785,22 +3044,22 @@
         <v>1</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2808,22 +3067,22 @@
         <v>1</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2831,22 +3090,22 @@
         <v>2</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2854,79 +3113,91 @@
         <v>2</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>6</v>
       </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
+      <c r="B52" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>242</v>
+      </c>
       <c r="D52" s="2" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>215</v>
+        <v>244</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>1</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="B53" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>248</v>
+      </c>
       <c r="D53" s="2" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>3</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="B54" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>242</v>
+      </c>
       <c r="D54" s="2" t="s">
-        <v>222</v>
+        <v>254</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2934,22 +3205,22 @@
         <v>1</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2957,22 +3228,22 @@
         <v>1</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>231</v>
+        <v>263</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>234</v>
+        <v>266</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>236</v>
+        <v>268</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2980,41 +3251,45 @@
         <v>4</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>238</v>
+        <v>270</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>240</v>
+        <v>272</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>6</v>
       </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="B58" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="D58" s="2" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>241</v>
+        <v>274</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>242</v>
+        <v>275</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3022,22 +3297,22 @@
         <v>1</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>244</v>
+        <v>276</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>246</v>
+        <v>278</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>247</v>
+        <v>279</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>244</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3045,22 +3320,22 @@
         <v>4</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>249</v>
+        <v>281</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>251</v>
+        <v>283</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>253</v>
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3068,22 +3343,22 @@
         <v>1</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>256</v>
+        <v>288</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>257</v>
+        <v>289</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>258</v>
+        <v>290</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3091,43 +3366,45 @@
         <v>2</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>259</v>
+        <v>291</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>260</v>
+        <v>292</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>261</v>
+        <v>293</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>262</v>
+        <v>294</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>259</v>
+        <v>291</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>1</v>
       </c>
-      <c r="B63" s="1"/>
+      <c r="B63" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="C63" s="2" t="s">
-        <v>263</v>
+        <v>296</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>264</v>
+        <v>297</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>265</v>
+        <v>298</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>266</v>
+        <v>299</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>265</v>
+        <v>298</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3135,22 +3412,22 @@
         <v>1</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>268</v>
+        <v>301</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>269</v>
+        <v>302</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>267</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3158,22 +3435,22 @@
         <v>2</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>270</v>
+        <v>303</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>271</v>
+        <v>304</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>272</v>
+        <v>305</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>274</v>
+        <v>307</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>270</v>
+        <v>303</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3181,526 +3458,574 @@
         <v>2</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>275</v>
+        <v>308</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>276</v>
+        <v>139</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>277</v>
+        <v>309</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>278</v>
+        <v>310</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>275</v>
+        <v>308</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>7</v>
       </c>
-      <c r="B67" s="1"/>
+      <c r="B67" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="C67" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>282</v>
+        <v>315</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>283</v>
+        <v>316</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>284</v>
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>11</v>
       </c>
-      <c r="B68" s="1"/>
+      <c r="B68" s="2" t="s">
+        <v>318</v>
+      </c>
       <c r="C68" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>285</v>
+        <v>319</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>286</v>
+        <v>320</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>287</v>
+        <v>321</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>19</v>
       </c>
-      <c r="B69" s="1"/>
+      <c r="B69" s="2" t="s">
+        <v>322</v>
+      </c>
       <c r="C69" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>288</v>
+        <v>323</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>289</v>
+        <v>324</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>32</v>
       </c>
-      <c r="B70" s="1"/>
+      <c r="B70" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="C70" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>291</v>
+        <v>327</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>292</v>
+        <v>328</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>293</v>
+        <v>329</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>20</v>
       </c>
-      <c r="B71" s="1"/>
+      <c r="B71" s="2" t="s">
+        <v>330</v>
+      </c>
       <c r="C71" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>294</v>
+        <v>331</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>296</v>
+        <v>333</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>26</v>
       </c>
-      <c r="B72" s="1"/>
+      <c r="B72" s="2" t="s">
+        <v>334</v>
+      </c>
       <c r="C72" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>297</v>
+        <v>335</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>298</v>
+        <v>336</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>299</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>1</v>
       </c>
-      <c r="B73" s="1"/>
+      <c r="B73" s="2" t="s">
+        <v>338</v>
+      </c>
       <c r="C73" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>300</v>
+        <v>339</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>301</v>
+        <v>340</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>302</v>
+        <v>341</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>1</v>
       </c>
-      <c r="B74" s="1"/>
+      <c r="B74" s="2" t="s">
+        <v>342</v>
+      </c>
       <c r="C74" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>303</v>
+        <v>343</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>304</v>
+        <v>344</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>296</v>
+        <v>333</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>16</v>
       </c>
-      <c r="B75" s="1"/>
+      <c r="B75" s="2" t="s">
+        <v>345</v>
+      </c>
       <c r="C75" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>305</v>
+        <v>346</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>306</v>
+        <v>347</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>307</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>9</v>
       </c>
-      <c r="B76" s="1"/>
+      <c r="B76" s="2" t="s">
+        <v>349</v>
+      </c>
       <c r="C76" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>308</v>
+        <v>350</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>309</v>
+        <v>351</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>299</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2</v>
       </c>
-      <c r="B77" s="1"/>
+      <c r="B77" s="2" t="s">
+        <v>352</v>
+      </c>
       <c r="C77" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>311</v>
+        <v>354</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>312</v>
+        <v>355</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>1</v>
       </c>
-      <c r="B78" s="1"/>
+      <c r="B78" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="C78" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>313</v>
+        <v>357</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>314</v>
+        <v>358</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>315</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>1</v>
       </c>
-      <c r="B79" s="1"/>
+      <c r="B79" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="C79" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>316</v>
+        <v>361</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>317</v>
+        <v>362</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>318</v>
+        <v>363</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>1</v>
       </c>
-      <c r="B80" s="1"/>
+      <c r="B80" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="C80" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>319</v>
+        <v>365</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>320</v>
+        <v>366</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>321</v>
+        <v>367</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>1</v>
       </c>
-      <c r="B81" s="1"/>
+      <c r="B81" s="2" t="s">
+        <v>368</v>
+      </c>
       <c r="C81" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>322</v>
+        <v>369</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>323</v>
+        <v>370</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>324</v>
+        <v>371</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>4</v>
       </c>
-      <c r="B82" s="1"/>
+      <c r="B82" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="C82" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>325</v>
+        <v>373</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>326</v>
+        <v>374</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>327</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>11</v>
       </c>
-      <c r="B83" s="1"/>
+      <c r="B83" s="2" t="s">
+        <v>376</v>
+      </c>
       <c r="C83" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>328</v>
+        <v>377</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>329</v>
+        <v>378</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>330</v>
+        <v>379</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>8</v>
       </c>
-      <c r="B84" s="1"/>
+      <c r="B84" s="2" t="s">
+        <v>380</v>
+      </c>
       <c r="C84" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>331</v>
+        <v>381</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>332</v>
+        <v>382</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>333</v>
+        <v>383</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>8</v>
       </c>
-      <c r="B85" s="1"/>
+      <c r="B85" s="2" t="s">
+        <v>384</v>
+      </c>
       <c r="C85" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>334</v>
+        <v>385</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>335</v>
+        <v>386</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>336</v>
+        <v>387</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>5</v>
       </c>
-      <c r="B86" s="1"/>
+      <c r="B86" s="2" t="s">
+        <v>388</v>
+      </c>
       <c r="C86" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>337</v>
+        <v>389</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>338</v>
+        <v>390</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>318</v>
+        <v>363</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>1</v>
       </c>
-      <c r="B87" s="1"/>
+      <c r="B87" s="2" t="s">
+        <v>391</v>
+      </c>
       <c r="C87" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>339</v>
+        <v>392</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>340</v>
+        <v>393</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>341</v>
+        <v>394</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>1</v>
       </c>
-      <c r="B88" s="1"/>
+      <c r="B88" s="2" t="s">
+        <v>395</v>
+      </c>
       <c r="C88" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>342</v>
+        <v>396</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>343</v>
+        <v>397</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>344</v>
+        <v>398</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>1</v>
       </c>
-      <c r="B89" s="1"/>
+      <c r="B89" s="2" t="s">
+        <v>399</v>
+      </c>
       <c r="C89" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>345</v>
+        <v>400</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>346</v>
+        <v>401</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>347</v>
+        <v>402</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>2</v>
       </c>
-      <c r="B90" s="1"/>
+      <c r="B90" s="2" t="s">
+        <v>403</v>
+      </c>
       <c r="C90" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>348</v>
+        <v>404</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>349</v>
+        <v>405</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>350</v>
+        <v>406</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3708,43 +4033,45 @@
         <v>2</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>351</v>
+        <v>407</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>352</v>
+        <v>408</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>353</v>
+        <v>409</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>354</v>
+        <v>410</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>355</v>
+        <v>411</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>351</v>
+        <v>407</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>2</v>
       </c>
-      <c r="B92" s="1"/>
+      <c r="B92" s="2" t="s">
+        <v>412</v>
+      </c>
       <c r="C92" s="2" t="s">
-        <v>356</v>
+        <v>413</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>357</v>
+        <v>414</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>358</v>
+        <v>415</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>359</v>
+        <v>416</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>360</v>
+        <v>412</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3752,22 +4079,22 @@
         <v>1</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>361</v>
+        <v>417</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>362</v>
+        <v>418</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>363</v>
+        <v>419</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>364</v>
+        <v>420</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>365</v>
+        <v>421</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>361</v>
+        <v>417</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3775,22 +4102,22 @@
         <v>41</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>366</v>
+        <v>422</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>367</v>
+        <v>423</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>368</v>
+        <v>424</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>369</v>
+        <v>425</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>370</v>
+        <v>426</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>366</v>
+        <v>422</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3798,60 +4125,68 @@
         <v>1</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>371</v>
+        <v>427</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>372</v>
+        <v>428</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>373</v>
+        <v>429</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>374</v>
+        <v>430</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>375</v>
+        <v>431</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>371</v>
+        <v>427</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>1</v>
       </c>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
+      <c r="B96" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>418</v>
+      </c>
       <c r="D96" s="2" t="s">
-        <v>376</v>
+        <v>433</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>377</v>
+        <v>434</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>378</v>
+        <v>435</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>379</v>
+        <v>432</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>1</v>
       </c>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
+      <c r="B97" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>418</v>
+      </c>
       <c r="D97" s="2" t="s">
-        <v>380</v>
+        <v>437</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>381</v>
+        <v>438</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>382</v>
+        <v>439</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>383</v>
+        <v>436</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3859,60 +4194,68 @@
         <v>1</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>384</v>
+        <v>440</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>385</v>
+        <v>441</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>386</v>
+        <v>442</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>387</v>
+        <v>443</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>388</v>
+        <v>444</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>384</v>
+        <v>440</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>3</v>
       </c>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
+      <c r="B99" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="D99" s="2" t="s">
-        <v>389</v>
+        <v>446</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>390</v>
+        <v>447</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>391</v>
+        <v>448</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>392</v>
+        <v>445</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>1</v>
       </c>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
+      <c r="B100" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>450</v>
+      </c>
       <c r="D100" s="2" t="s">
-        <v>393</v>
+        <v>451</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>394</v>
+        <v>452</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>395</v>
+        <v>453</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>396</v>
+        <v>454</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3920,22 +4263,22 @@
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>397</v>
+        <v>455</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>398</v>
+        <v>456</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>399</v>
+        <v>457</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>400</v>
+        <v>458</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>401</v>
+        <v>459</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>397</v>
+        <v>455</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3943,22 +4286,22 @@
         <v>1</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>402</v>
+        <v>460</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>403</v>
+        <v>461</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>404</v>
+        <v>462</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>405</v>
+        <v>463</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>406</v>
+        <v>464</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>402</v>
+        <v>460</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3966,22 +4309,22 @@
         <v>1</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>407</v>
+        <v>465</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>408</v>
+        <v>466</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>409</v>
+        <v>467</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>410</v>
+        <v>468</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>411</v>
+        <v>469</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>407</v>
+        <v>465</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3989,62 +4332,68 @@
         <v>1</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>412</v>
+        <v>470</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>408</v>
+        <v>466</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>413</v>
+        <v>471</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>414</v>
+        <v>472</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>415</v>
+        <v>473</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>412</v>
+        <v>470</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>1</v>
       </c>
-      <c r="B105" s="1"/>
+      <c r="B105" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="C105" s="2" t="s">
-        <v>416</v>
+        <v>475</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>417</v>
+        <v>476</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>418</v>
+        <v>477</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>419</v>
+        <v>478</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>420</v>
+        <v>474</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>1</v>
       </c>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
+      <c r="B106" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>480</v>
+      </c>
       <c r="D106" s="2" t="s">
-        <v>421</v>
+        <v>481</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>422</v>
+        <v>482</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>423</v>
+        <v>483</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>424</v>
+        <v>479</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4052,22 +4401,22 @@
         <v>1</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>425</v>
+        <v>484</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>426</v>
+        <v>485</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>427</v>
+        <v>486</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>428</v>
+        <v>487</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>429</v>
+        <v>488</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>425</v>
+        <v>484</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4075,22 +4424,22 @@
         <v>1</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>430</v>
+        <v>489</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>431</v>
+        <v>490</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>432</v>
+        <v>491</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>433</v>
+        <v>492</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>434</v>
+        <v>493</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>430</v>
+        <v>489</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4098,22 +4447,22 @@
         <v>1</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>435</v>
+        <v>494</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>249</v>
+        <v>281</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>436</v>
+        <v>495</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>437</v>
+        <v>496</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>438</v>
+        <v>497</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>435</v>
+        <v>494</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4121,22 +4470,22 @@
         <v>1</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>439</v>
+        <v>498</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>440</v>
+        <v>499</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>441</v>
+        <v>500</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>442</v>
+        <v>501</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>443</v>
+        <v>502</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>444</v>
+        <v>503</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4144,22 +4493,22 @@
         <v>1</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>445</v>
+        <v>504</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>446</v>
+        <v>505</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>447</v>
+        <v>506</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>448</v>
+        <v>507</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>449</v>
+        <v>508</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>450</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change R9 to FITTED Change R10 to NOT_FITTED Changed B3B-XH-A(LF)(SN) to B4B-XH-A(LF)(SN)
</commit_message>
<xml_diff>
--- a/Project Outputs for Longboard_32bit/BOM/JLPCB BOM-Longboard_32bit_A4_FULL_PLACE.xlsx
+++ b/Project Outputs for Longboard_32bit/BOM/JLPCB BOM-Longboard_32bit_A4_FULL_PLACE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sienci\Repos\longboard_stm32\Project Outputs for Longboard_32bit\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{546D7A82-C289-42EC-B9F7-9585D5359C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FBE9B29-85D1-4300-A5F3-3A82486A0F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84855" yWindow="2715" windowWidth="28800" windowHeight="15195" xr2:uid="{5CB1C09F-25AA-42A5-9CE5-4242CA91869C}"/>
+    <workbookView xWindow="81570" yWindow="2475" windowWidth="28800" windowHeight="15195" xr2:uid="{ADF552B5-F118-4D94-BAA8-A9C1B1B350D1}"/>
   </bookViews>
   <sheets>
     <sheet name="JLPCB BOM-Longboard_32bit_A4_FU" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="515">
   <si>
     <t>Quantity</t>
   </si>
@@ -546,6 +546,147 @@
     <t>J3, J13</t>
   </si>
   <si>
+    <t>B4B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>XH Series 4 Position 2.5 mm Pitch Through Hole Crimp Top Entry Shrouded Header</t>
+  </si>
+  <si>
+    <t>C144395</t>
+  </si>
+  <si>
+    <t>J4, J5, J6, J7, J8</t>
+  </si>
+  <si>
+    <t>WJ15EDGRC-3.81-5P</t>
+  </si>
+  <si>
+    <t>Ningbo Kangnex</t>
+  </si>
+  <si>
+    <t>3.81mm Green Board Edge/Receptacle-Close Push-Pull,P=3.81mm Pluggable System Terminal Block ROHS</t>
+  </si>
+  <si>
+    <t>C8395</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>WJ15EDGRC-3.81-4P</t>
+  </si>
+  <si>
+    <t>Ningbo Kangnex Elec</t>
+  </si>
+  <si>
+    <t>C7245</t>
+  </si>
+  <si>
+    <t>J10, J34</t>
+  </si>
+  <si>
+    <t>WJ15EDGRC-3.81-3P</t>
+  </si>
+  <si>
+    <t>C8406</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>DS1133-S60BPX</t>
+  </si>
+  <si>
+    <t>CONNFLY Elec</t>
+  </si>
+  <si>
+    <t>RJ12 RJReceptacle 1 Plugin Ethernet Connectors/Modular Connectors (RJ45 RJ11) ROHS</t>
+  </si>
+  <si>
+    <t>C77859</t>
+  </si>
+  <si>
+    <t>J12, J14</t>
+  </si>
+  <si>
+    <t>907-111A1022D10200</t>
+  </si>
+  <si>
+    <t>Jing Extension of the Electronic Co.</t>
+  </si>
+  <si>
+    <t>USB 2.0 2 8 Female Type-A Plugin USB Connectors ROHS</t>
+  </si>
+  <si>
+    <t>C12049</t>
+  </si>
+  <si>
+    <t>J15, J16</t>
+  </si>
+  <si>
+    <t>10118194-0001LF</t>
+  </si>
+  <si>
+    <t>Amphenol ICC (FCI)</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB2.0 MICRO B SMD R/A</t>
+  </si>
+  <si>
+    <t>C132563</t>
+  </si>
+  <si>
+    <t>J17</t>
+  </si>
+  <si>
+    <t>ARJM11D7-502-AB-EW2</t>
+  </si>
+  <si>
+    <t>Abracon LLC</t>
+  </si>
+  <si>
+    <t>1 Port RJ45Through Hole 10/100/1000 Base-T, AutoMDIX</t>
+  </si>
+  <si>
+    <t>535-14152-ND</t>
+  </si>
+  <si>
+    <t>J18</t>
+  </si>
+  <si>
+    <t>1747981-1</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>HDMI Receptacle, Pitch 0.5 mm, 19 Position, Height 6.38 mm, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>C428484</t>
+  </si>
+  <si>
+    <t>J19</t>
+  </si>
+  <si>
+    <t>TYPE-C-31-M-12</t>
+  </si>
+  <si>
+    <t>HRO Electronics Co., Ltd.</t>
+  </si>
+  <si>
+    <t>USB Connectors 24 Receptacle 1 8.94*7.3mm RoHS</t>
+  </si>
+  <si>
+    <t>C2765186</t>
+  </si>
+  <si>
+    <t>J20</t>
+  </si>
+  <si>
     <t>B3B-XH-A(LF)(SN)</t>
   </si>
   <si>
@@ -558,133 +699,7 @@
     <t>C144394</t>
   </si>
   <si>
-    <t>J4, J5, J6, J7, J8, J21</t>
-  </si>
-  <si>
-    <t>WJ15EDGRC-3.81-5P</t>
-  </si>
-  <si>
-    <t>Ningbo Kangnex</t>
-  </si>
-  <si>
-    <t>3.81mm Green Board Edge/Receptacle-Close Push-Pull,P=3.81mm Pluggable System Terminal Block ROHS</t>
-  </si>
-  <si>
-    <t>C8395</t>
-  </si>
-  <si>
-    <t>J9</t>
-  </si>
-  <si>
-    <t>WJ15EDGRC-3.81-4P</t>
-  </si>
-  <si>
-    <t>Ningbo Kangnex Elec</t>
-  </si>
-  <si>
-    <t>C7245</t>
-  </si>
-  <si>
-    <t>J10, J34</t>
-  </si>
-  <si>
-    <t>WJ15EDGRC-3.81-3P</t>
-  </si>
-  <si>
-    <t>C8406</t>
-  </si>
-  <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>DS1133-S60BPX</t>
-  </si>
-  <si>
-    <t>CONNFLY Elec</t>
-  </si>
-  <si>
-    <t>RJ12 RJReceptacle 1 Plugin Ethernet Connectors/Modular Connectors (RJ45 RJ11) ROHS</t>
-  </si>
-  <si>
-    <t>C77859</t>
-  </si>
-  <si>
-    <t>J12, J14</t>
-  </si>
-  <si>
-    <t>907-111A1022D10200</t>
-  </si>
-  <si>
-    <t>Jing Extension of the Electronic Co.</t>
-  </si>
-  <si>
-    <t>USB 2.0 2 8 Female Type-A Plugin USB Connectors ROHS</t>
-  </si>
-  <si>
-    <t>C12049</t>
-  </si>
-  <si>
-    <t>J15, J16</t>
-  </si>
-  <si>
-    <t>10118194-0001LF</t>
-  </si>
-  <si>
-    <t>Amphenol ICC (FCI)</t>
-  </si>
-  <si>
-    <t>CONN RCPT USB2.0 MICRO B SMD R/A</t>
-  </si>
-  <si>
-    <t>C132563</t>
-  </si>
-  <si>
-    <t>J17</t>
-  </si>
-  <si>
-    <t>ARJM11D7-502-AB-EW2</t>
-  </si>
-  <si>
-    <t>Abracon LLC</t>
-  </si>
-  <si>
-    <t>1 Port RJ45Through Hole 10/100/1000 Base-T, AutoMDIX</t>
-  </si>
-  <si>
-    <t>535-14152-ND</t>
-  </si>
-  <si>
-    <t>J18</t>
-  </si>
-  <si>
-    <t>1747981-1</t>
-  </si>
-  <si>
-    <t>TE Connectivity</t>
-  </si>
-  <si>
-    <t>HDMI Receptacle, Pitch 0.5 mm, 19 Position, Height 6.38 mm, RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>C428484</t>
-  </si>
-  <si>
-    <t>J19</t>
-  </si>
-  <si>
-    <t>TYPE-C-31-M-12</t>
-  </si>
-  <si>
-    <t>HRO Electronics Co., Ltd.</t>
-  </si>
-  <si>
-    <t>USB Connectors 24 Receptacle 1 8.94*7.3mm RoHS</t>
-  </si>
-  <si>
-    <t>C2765186</t>
-  </si>
-  <si>
-    <t>J20</t>
+    <t>J21</t>
   </si>
   <si>
     <t>WJ2EDGK-5.08-4P</t>
@@ -987,7 +1002,7 @@
     <t>C21189</t>
   </si>
   <si>
-    <t>R2, R3, R4, R10, R130_AX_TR1, R130_AX_TR2, R131</t>
+    <t>R2, R3, R4, R9, R130_AX_TR1, R130_AX_TR2, R131</t>
   </si>
   <si>
     <t>0Ω ±1%</t>
@@ -1942,8 +1957,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514EB639-7DF3-447A-8364-0B606F89ECCF}">
-  <dimension ref="A1:G111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E60BE0-DD33-4440-B2DA-BCB9881CF95D}">
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2765,7 +2780,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>169</v>
@@ -2995,7 +3010,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>216</v>
@@ -3018,22 +3033,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>221</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>221</v>
@@ -3041,25 +3056,25 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>180</v>
+        <v>222</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3067,36 +3082,36 @@
         <v>1</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E49" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>235</v>
@@ -3105,7 +3120,7 @@
         <v>236</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3116,16 +3131,16 @@
         <v>237</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>161</v>
+        <v>238</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>237</v>
@@ -3133,13 +3148,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>242</v>
+        <v>161</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>243</v>
@@ -3151,41 +3166,41 @@
         <v>245</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>254</v>
@@ -3202,25 +3217,25 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>258</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3243,18 +3258,18 @@
         <v>267</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>270</v>
@@ -3266,64 +3281,64 @@
         <v>272</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>176</v>
+        <v>275</v>
       </c>
       <c r="E58" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>277</v>
+        <v>176</v>
       </c>
       <c r="E59" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>281</v>
+        <v>161</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>282</v>
@@ -3335,50 +3350,50 @@
         <v>284</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>291</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>233</v>
+        <v>292</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>291</v>
@@ -3386,13 +3401,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>296</v>
+        <v>238</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>297</v>
@@ -3404,7 +3419,7 @@
         <v>299</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3415,33 +3430,33 @@
         <v>300</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>217</v>
+        <v>301</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>226</v>
+        <v>302</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>304</v>
+        <v>222</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>305</v>
+        <v>231</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>306</v>
@@ -3450,7 +3465,7 @@
         <v>307</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3461,16 +3476,16 @@
         <v>308</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>139</v>
+        <v>309</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>308</v>
@@ -3478,13 +3493,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>313</v>
+        <v>139</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>314</v>
@@ -3496,145 +3511,145 @@
         <v>316</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="D68" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3642,114 +3657,114 @@
         <v>1</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>337</v>
+        <v>353</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3757,22 +3772,22 @@
         <v>1</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3780,22 +3795,22 @@
         <v>1</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3803,91 +3818,91 @@
         <v>1</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3895,68 +3910,68 @@
         <v>8</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>363</v>
+        <v>392</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>394</v>
+        <v>368</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3964,22 +3979,22 @@
         <v>1</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3987,45 +4002,45 @@
         <v>1</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4033,22 +4048,22 @@
         <v>2</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>408</v>
+        <v>318</v>
       </c>
       <c r="D91" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="F91" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="G91" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4076,7 +4091,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>417</v>
@@ -4099,7 +4114,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>422</v>
@@ -4122,7 +4137,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>427</v>
@@ -4151,16 +4166,16 @@
         <v>432</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>418</v>
+        <v>433</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>432</v>
@@ -4171,22 +4186,22 @@
         <v>1</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="D97" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G97" s="2" t="s">
         <v>437</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4194,10 +4209,10 @@
         <v>1</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>442</v>
@@ -4209,27 +4224,27 @@
         <v>444</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>445</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>85</v>
+        <v>446</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>445</v>
@@ -4237,13 +4252,13 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>450</v>
+        <v>85</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>451</v>
@@ -4255,7 +4270,7 @@
         <v>453</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -4263,22 +4278,22 @@
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="E101" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="G101" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -4335,16 +4350,16 @@
         <v>470</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>470</v>
@@ -4355,10 +4370,10 @@
         <v>1</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>476</v>
@@ -4370,7 +4385,7 @@
         <v>478</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4450,16 +4465,16 @@
         <v>494</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>281</v>
+        <v>495</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>494</v>
@@ -4470,10 +4485,10 @@
         <v>1</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>499</v>
+        <v>286</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>500</v>
@@ -4485,7 +4500,7 @@
         <v>502</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4493,22 +4508,45 @@
         <v>1</v>
       </c>
       <c r="B111" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="E111" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="F111" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="G111" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="G111" s="2" t="s">
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>1</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>509</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>